<commit_message>
Regret addition to greedy cycle
</commit_message>
<xml_diff>
--- a/EvolutionaryComputation/out/production/EvolutionaryComputation/Solution checker.xlsx
+++ b/EvolutionaryComputation/out/production/EvolutionaryComputation/Solution checker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tymon\OneDrive\Pulpit\University\Sem7\EvolutionaryComputation\Labs\EvolutionaryComputation\EvolutionaryComputation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4F0E1D-164A-4C96-925E-2FCCAA4759C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513C5756-300E-471B-92A3-0E4E70603EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TSPA" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,18 +81,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="7"/>
-      <color rgb="FFD6DEEB"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,13 +118,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -398,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K202"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D202"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -440,15 +454,15 @@
       <c r="F2" s="1"/>
       <c r="I2" s="2">
         <f>SUM(I3:I102)</f>
-        <v>99670</v>
+        <v>47910</v>
       </c>
       <c r="J2" s="2">
         <f>SUM(J3:J102)</f>
-        <v>165696</v>
+        <v>23578</v>
       </c>
       <c r="K2" s="2">
         <f>I2+J2</f>
-        <v>265366</v>
+        <v>71488</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -464,24 +478,24 @@
       <c r="D3">
         <v>496</v>
       </c>
-      <c r="F3">
-        <v>31</v>
+      <c r="F3" s="4">
+        <v>0</v>
       </c>
       <c r="G3">
         <f>LOOKUP($F3,$A$3:$A$202,B$3:B$202)</f>
-        <v>3697</v>
+        <v>1355</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:I3" si="0">LOOKUP($F3,$A$3:$A$202,C$3:C$202)</f>
-        <v>324</v>
+        <v>1796</v>
       </c>
       <c r="I3">
         <f t="shared" si="0"/>
-        <v>394</v>
+        <v>496</v>
       </c>
       <c r="J3">
         <f>INT(SQRT((G3-G4)*(G3-G4)+(H3-H4)*(H3-H4)) +0.5)</f>
-        <v>1311</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -497,24 +511,24 @@
       <c r="D4">
         <v>414</v>
       </c>
-      <c r="F4">
-        <v>111</v>
+      <c r="F4" s="4">
+        <v>117</v>
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G67" si="1">LOOKUP($F4,$A$3:$A$202,B$3:B$202)</f>
-        <v>2559</v>
+        <v>1199</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H67" si="2">LOOKUP($F4,$A$3:$A$202,C$3:C$202)</f>
-        <v>975</v>
+        <v>1948</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I67" si="3">LOOKUP($F4,$A$3:$A$202,D$3:D$202)</f>
-        <v>1478</v>
+        <v>611</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J67" si="4">INT(SQRT((G4-G5)*(G4-G5)+(H4-H5)*(H4-H5)) +0.5)</f>
-        <v>733</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -530,24 +544,24 @@
       <c r="D5">
         <v>500</v>
       </c>
-      <c r="F5">
-        <v>14</v>
+      <c r="F5" s="4">
+        <v>143</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>3088</v>
+        <v>1417</v>
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
-        <v>1482</v>
+        <v>1961</v>
       </c>
       <c r="I5">
         <f t="shared" si="3"/>
-        <v>267</v>
+        <v>424</v>
       </c>
       <c r="J5">
         <f t="shared" si="4"/>
-        <v>1406</v>
+        <v>421</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -563,24 +577,24 @@
       <c r="D6">
         <v>1133</v>
       </c>
-      <c r="F6">
-        <v>80</v>
+      <c r="F6" s="4">
+        <v>183</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>1823</v>
+        <v>1838</v>
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>868</v>
+        <v>1943</v>
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
-        <v>445</v>
+        <v>43</v>
       </c>
       <c r="J6">
         <f t="shared" si="4"/>
-        <v>2025</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -596,24 +610,24 @@
       <c r="D7">
         <v>903</v>
       </c>
-      <c r="F7">
-        <v>95</v>
+      <c r="F7" s="4">
+        <v>89</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>3691</v>
+        <v>1922</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>1650</v>
+        <v>1845</v>
       </c>
       <c r="I7">
         <f t="shared" si="3"/>
-        <v>1075</v>
+        <v>754</v>
       </c>
       <c r="J7">
         <f t="shared" si="4"/>
-        <v>784</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -629,24 +643,24 @@
       <c r="D8">
         <v>1081</v>
       </c>
-      <c r="F8">
-        <v>169</v>
+      <c r="F8" s="4">
+        <v>186</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>3661</v>
+        <v>2121</v>
       </c>
       <c r="H8">
         <f t="shared" si="2"/>
-        <v>867</v>
+        <v>1641</v>
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
-        <v>1528</v>
+        <v>859</v>
       </c>
       <c r="J8">
         <f t="shared" si="4"/>
-        <v>408</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -662,24 +676,24 @@
       <c r="D9">
         <v>1859</v>
       </c>
-      <c r="F9">
-        <v>8</v>
+      <c r="F9" s="4">
+        <v>23</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>3474</v>
+        <v>2005</v>
       </c>
       <c r="H9">
         <f t="shared" si="2"/>
-        <v>1230</v>
+        <v>1631</v>
       </c>
       <c r="I9">
         <f t="shared" si="3"/>
-        <v>1389</v>
+        <v>819</v>
       </c>
       <c r="J9">
         <f t="shared" si="4"/>
-        <v>1398</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -695,24 +709,24 @@
       <c r="D10">
         <v>945</v>
       </c>
-      <c r="F10">
-        <v>26</v>
+      <c r="F10" s="4">
+        <v>137</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>2371</v>
+        <v>1902</v>
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
-        <v>371</v>
+        <v>1390</v>
       </c>
       <c r="I10">
         <f t="shared" si="3"/>
-        <v>834</v>
+        <v>293</v>
       </c>
       <c r="J10">
         <f t="shared" si="4"/>
-        <v>837</v>
+        <v>392</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -728,24 +742,24 @@
       <c r="D11">
         <v>1389</v>
       </c>
-      <c r="F11">
-        <v>92</v>
+      <c r="F11" s="4">
+        <v>176</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>3174</v>
+        <v>1774</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
-        <v>606</v>
+        <v>1020</v>
       </c>
       <c r="I11">
         <f t="shared" si="3"/>
-        <v>390</v>
+        <v>70</v>
       </c>
       <c r="J11">
         <f t="shared" si="4"/>
-        <v>2948</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -761,24 +775,24 @@
       <c r="D12">
         <v>776</v>
       </c>
-      <c r="F12">
-        <v>48</v>
+      <c r="F12" s="4">
+        <v>80</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>227</v>
+        <v>1823</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
-        <v>534</v>
+        <v>868</v>
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
-        <v>986</v>
+        <v>445</v>
       </c>
       <c r="J12">
         <f t="shared" si="4"/>
-        <v>3007</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -794,24 +808,24 @@
       <c r="D13">
         <v>774</v>
       </c>
-      <c r="F13">
-        <v>106</v>
+      <c r="F13" s="4">
+        <v>79</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>3171</v>
+        <v>1852</v>
       </c>
       <c r="H13">
         <f t="shared" si="2"/>
-        <v>1147</v>
+        <v>682</v>
       </c>
       <c r="I13">
         <f t="shared" si="3"/>
-        <v>264</v>
+        <v>561</v>
       </c>
       <c r="J13">
         <f t="shared" si="4"/>
-        <v>2903</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -827,24 +841,24 @@
       <c r="D14">
         <v>1727</v>
       </c>
-      <c r="F14">
-        <v>160</v>
+      <c r="F14" s="4">
+        <v>63</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>307</v>
+        <v>1972</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>671</v>
+        <v>616</v>
       </c>
       <c r="I14">
         <f t="shared" si="3"/>
-        <v>228</v>
+        <v>129</v>
       </c>
       <c r="J14">
         <f t="shared" si="4"/>
-        <v>471</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -860,24 +874,24 @@
       <c r="D15">
         <v>1370</v>
       </c>
-      <c r="F15">
-        <v>11</v>
+      <c r="F15" s="4">
+        <v>94</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>681</v>
+        <v>2237</v>
       </c>
       <c r="H15">
         <f t="shared" si="2"/>
-        <v>385</v>
+        <v>764</v>
       </c>
       <c r="I15">
         <f t="shared" si="3"/>
-        <v>1727</v>
+        <v>323</v>
       </c>
       <c r="J15">
         <f t="shared" si="4"/>
-        <v>1876</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -893,24 +907,24 @@
       <c r="D16">
         <v>1839</v>
       </c>
-      <c r="F16">
-        <v>152</v>
+      <c r="F16" s="4">
+        <v>124</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>2549</v>
+        <v>2337</v>
       </c>
       <c r="H16">
         <f t="shared" si="2"/>
-        <v>554</v>
+        <v>850</v>
       </c>
       <c r="I16">
         <f t="shared" si="3"/>
-        <v>351</v>
+        <v>962</v>
       </c>
       <c r="J16">
         <f t="shared" si="4"/>
-        <v>492</v>
+        <v>364</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -926,24 +940,24 @@
       <c r="D17">
         <v>267</v>
       </c>
-      <c r="F17">
-        <v>130</v>
+      <c r="F17" s="4">
+        <v>152</v>
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>2207</v>
+        <v>2549</v>
       </c>
       <c r="H17">
         <f t="shared" si="2"/>
-        <v>907</v>
+        <v>554</v>
       </c>
       <c r="I17">
         <f t="shared" si="3"/>
-        <v>1687</v>
+        <v>351</v>
       </c>
       <c r="J17">
         <f t="shared" si="4"/>
-        <v>1397</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -959,24 +973,24 @@
       <c r="D18">
         <v>891</v>
       </c>
-      <c r="F18">
-        <v>119</v>
+      <c r="F18" s="4">
+        <v>97</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>3587</v>
+        <v>2465</v>
       </c>
       <c r="H18">
         <f t="shared" si="2"/>
-        <v>1123</v>
+        <v>426</v>
       </c>
       <c r="I18">
         <f t="shared" si="3"/>
-        <v>1064</v>
+        <v>310</v>
       </c>
       <c r="J18">
         <f t="shared" si="4"/>
-        <v>2178</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -992,24 +1006,24 @@
       <c r="D19">
         <v>82</v>
       </c>
-      <c r="F19">
-        <v>109</v>
+      <c r="F19" s="4">
+        <v>1</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>1410</v>
+        <v>2524</v>
       </c>
       <c r="H19">
         <f t="shared" si="2"/>
-        <v>1050</v>
+        <v>387</v>
       </c>
       <c r="I19">
         <f t="shared" si="3"/>
-        <v>1326</v>
+        <v>414</v>
       </c>
       <c r="J19">
         <f t="shared" si="4"/>
-        <v>1008</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -1025,24 +1039,24 @@
       <c r="D20">
         <v>1819</v>
       </c>
-      <c r="F20">
-        <v>189</v>
+      <c r="F20" s="4">
+        <v>101</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>2298</v>
+        <v>2504</v>
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
-        <v>573</v>
+        <v>302</v>
       </c>
       <c r="I20">
         <f t="shared" si="3"/>
-        <v>1226</v>
+        <v>297</v>
       </c>
       <c r="J20">
         <f t="shared" si="4"/>
-        <v>543</v>
+        <v>294</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -1058,24 +1072,24 @@
       <c r="D21">
         <v>182</v>
       </c>
-      <c r="F21">
-        <v>75</v>
+      <c r="F21" s="4">
+        <v>2</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>2614</v>
+        <v>2769</v>
       </c>
       <c r="H21">
         <f t="shared" si="2"/>
-        <v>132</v>
+        <v>430</v>
       </c>
       <c r="I21">
         <f t="shared" si="3"/>
-        <v>360</v>
+        <v>500</v>
       </c>
       <c r="J21">
         <f t="shared" si="4"/>
-        <v>270</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -1091,24 +1105,24 @@
       <c r="D22">
         <v>1500</v>
       </c>
-      <c r="F22">
-        <v>1</v>
+      <c r="F22" s="4">
+        <v>120</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>2524</v>
+        <v>3016</v>
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
-        <v>387</v>
+        <v>260</v>
       </c>
       <c r="I22">
         <f t="shared" si="3"/>
-        <v>414</v>
+        <v>34</v>
       </c>
       <c r="J22">
         <f t="shared" si="4"/>
-        <v>2268</v>
+        <v>297</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -1124,24 +1138,24 @@
       <c r="D23">
         <v>1371</v>
       </c>
-      <c r="F23">
-        <v>177</v>
+      <c r="F23" s="4">
+        <v>129</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>263</v>
+        <v>3023</v>
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
-        <v>208</v>
+        <v>557</v>
       </c>
       <c r="I23">
         <f t="shared" si="3"/>
-        <v>527</v>
+        <v>657</v>
       </c>
       <c r="J23">
         <f t="shared" si="4"/>
-        <v>1072</v>
+        <v>386</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -1157,24 +1171,24 @@
       <c r="D24">
         <v>774</v>
       </c>
-      <c r="F24">
-        <v>41</v>
+      <c r="F24" s="4">
+        <v>55</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>550</v>
+        <v>3144</v>
       </c>
       <c r="H24">
         <f t="shared" si="2"/>
-        <v>1241</v>
+        <v>924</v>
       </c>
       <c r="I24">
         <f t="shared" si="3"/>
-        <v>379</v>
+        <v>585</v>
       </c>
       <c r="J24">
         <f t="shared" si="4"/>
-        <v>1360</v>
+        <v>463</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
@@ -1190,24 +1204,24 @@
       <c r="D25">
         <v>88</v>
       </c>
-      <c r="F25">
-        <v>137</v>
+      <c r="F25" s="4">
+        <v>49</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>1902</v>
+        <v>2943</v>
       </c>
       <c r="H25">
         <f t="shared" si="2"/>
-        <v>1390</v>
+        <v>1341</v>
       </c>
       <c r="I25">
         <f t="shared" si="3"/>
-        <v>293</v>
+        <v>104</v>
       </c>
       <c r="J25">
         <f t="shared" si="4"/>
-        <v>1937</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -1223,24 +1237,24 @@
       <c r="D26">
         <v>819</v>
       </c>
-      <c r="F26">
-        <v>174</v>
+      <c r="F26" s="4">
+        <v>102</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
-        <v>3797</v>
+        <v>2866</v>
       </c>
       <c r="H26">
         <f t="shared" si="2"/>
-        <v>990</v>
+        <v>1409</v>
       </c>
       <c r="I26">
         <f t="shared" si="3"/>
-        <v>1716</v>
+        <v>939</v>
       </c>
       <c r="J26">
         <f t="shared" si="4"/>
-        <v>3600</v>
+        <v>421</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -1256,24 +1270,24 @@
       <c r="D27">
         <v>1481</v>
       </c>
-      <c r="F27">
-        <v>199</v>
+      <c r="F27" s="4">
+        <v>148</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
-        <v>262</v>
+        <v>2498</v>
       </c>
       <c r="H27">
         <f t="shared" si="2"/>
-        <v>1669</v>
+        <v>1204</v>
       </c>
       <c r="I27">
         <f t="shared" si="3"/>
-        <v>1307</v>
+        <v>450</v>
       </c>
       <c r="J27">
         <f t="shared" si="4"/>
-        <v>2679</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -1289,24 +1303,24 @@
       <c r="D28">
         <v>756</v>
       </c>
-      <c r="F28">
-        <v>150</v>
+      <c r="F28" s="4">
+        <v>9</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
-        <v>2540</v>
+        <v>2662</v>
       </c>
       <c r="H28">
         <f t="shared" si="2"/>
-        <v>260</v>
+        <v>1405</v>
       </c>
       <c r="I28">
         <f t="shared" si="3"/>
-        <v>1935</v>
+        <v>776</v>
       </c>
       <c r="J28">
         <f t="shared" si="4"/>
-        <v>2256</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -1322,24 +1336,24 @@
       <c r="D29">
         <v>834</v>
       </c>
-      <c r="F29">
-        <v>192</v>
+      <c r="F29" s="4">
+        <v>62</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
-        <v>350</v>
+        <v>2678</v>
       </c>
       <c r="H29">
         <f t="shared" si="2"/>
-        <v>802</v>
+        <v>1417</v>
       </c>
       <c r="I29">
         <f t="shared" si="3"/>
-        <v>1689</v>
+        <v>182</v>
       </c>
       <c r="J29">
         <f t="shared" si="4"/>
-        <v>3557</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -1355,24 +1369,24 @@
       <c r="D30">
         <v>974</v>
       </c>
-      <c r="F30">
-        <v>175</v>
+      <c r="F30" s="4">
+        <v>144</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
-        <v>3828</v>
+        <v>2898</v>
       </c>
       <c r="H30">
         <f t="shared" si="2"/>
-        <v>57</v>
+        <v>1609</v>
       </c>
       <c r="I30">
         <f t="shared" si="3"/>
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="J30">
         <f t="shared" si="4"/>
-        <v>2283</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -1388,24 +1402,24 @@
       <c r="D31">
         <v>1477</v>
       </c>
-      <c r="F31">
-        <v>114</v>
+      <c r="F31" s="4">
+        <v>14</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>2286</v>
+        <v>3088</v>
       </c>
       <c r="H31">
         <f t="shared" si="2"/>
-        <v>1740</v>
+        <v>1482</v>
       </c>
       <c r="I31">
         <f t="shared" si="3"/>
-        <v>1022</v>
+        <v>267</v>
       </c>
       <c r="J31">
         <f t="shared" si="4"/>
-        <v>2318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
@@ -1421,24 +1435,24 @@
       <c r="D32">
         <v>1499</v>
       </c>
-      <c r="F32">
-        <v>4</v>
+      <c r="F32" s="4">
+        <v>178</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
-        <v>661</v>
+        <v>3134</v>
       </c>
       <c r="H32">
         <f t="shared" si="2"/>
-        <v>87</v>
+        <v>1169</v>
       </c>
       <c r="I32">
         <f t="shared" si="3"/>
-        <v>903</v>
+        <v>420</v>
       </c>
       <c r="J32">
         <f t="shared" si="4"/>
-        <v>628</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
@@ -1454,24 +1468,24 @@
       <c r="D33">
         <v>1025</v>
       </c>
-      <c r="F33">
-        <v>77</v>
+      <c r="F33" s="4">
+        <v>106</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
-        <v>816</v>
+        <v>3171</v>
       </c>
       <c r="H33">
         <f t="shared" si="2"/>
-        <v>696</v>
+        <v>1147</v>
       </c>
       <c r="I33">
         <f t="shared" si="3"/>
-        <v>1351</v>
+        <v>264</v>
       </c>
       <c r="J33">
         <f t="shared" si="4"/>
-        <v>115</v>
+        <v>429</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
@@ -1487,24 +1501,24 @@
       <c r="D34">
         <v>394</v>
       </c>
-      <c r="F34">
-        <v>43</v>
+      <c r="F34" s="4">
+        <v>165</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
-        <v>724</v>
+        <v>3576</v>
       </c>
       <c r="H34">
         <f t="shared" si="2"/>
-        <v>765</v>
+        <v>1287</v>
       </c>
       <c r="I34">
         <f t="shared" si="3"/>
-        <v>581</v>
+        <v>286</v>
       </c>
       <c r="J34">
         <f t="shared" si="4"/>
-        <v>1531</v>
+        <v>415</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
@@ -1520,24 +1534,24 @@
       <c r="D35">
         <v>1585</v>
       </c>
-      <c r="F35">
-        <v>121</v>
+      <c r="F35" s="4">
+        <v>90</v>
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
-        <v>2218</v>
+        <v>3991</v>
       </c>
       <c r="H35">
         <f t="shared" si="2"/>
-        <v>431</v>
+        <v>1300</v>
       </c>
       <c r="I35">
         <f t="shared" si="3"/>
-        <v>1094</v>
+        <v>246</v>
       </c>
       <c r="J35">
         <f t="shared" si="4"/>
-        <v>1252</v>
+        <v>460</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
@@ -1553,24 +1567,24 @@
       <c r="D36">
         <v>1855</v>
       </c>
-      <c r="F36">
-        <v>91</v>
+      <c r="F36" s="4">
+        <v>81</v>
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
-        <v>3430</v>
+        <v>3901</v>
       </c>
       <c r="H36">
         <f t="shared" si="2"/>
-        <v>746</v>
+        <v>849</v>
       </c>
       <c r="I36">
         <f t="shared" si="3"/>
-        <v>1510</v>
+        <v>606</v>
       </c>
       <c r="J36">
         <f t="shared" si="4"/>
-        <v>643</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
@@ -1586,24 +1600,24 @@
       <c r="D37">
         <v>191</v>
       </c>
-      <c r="F37">
-        <v>50</v>
+      <c r="F37" s="4">
+        <v>196</v>
       </c>
       <c r="G37">
         <f t="shared" si="1"/>
-        <v>3846</v>
+        <v>3688</v>
       </c>
       <c r="H37">
         <f t="shared" si="2"/>
-        <v>256</v>
+        <v>759</v>
       </c>
       <c r="I37">
         <f t="shared" si="3"/>
-        <v>1947</v>
+        <v>727</v>
       </c>
       <c r="J37">
         <f t="shared" si="4"/>
-        <v>2871</v>
+        <v>365</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
@@ -1619,24 +1633,24 @@
       <c r="D38">
         <v>976</v>
       </c>
-      <c r="F38">
-        <v>149</v>
+      <c r="F38" s="4">
+        <v>40</v>
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
-        <v>993</v>
+        <v>3585</v>
       </c>
       <c r="H38">
         <f t="shared" si="2"/>
-        <v>581</v>
+        <v>1109</v>
       </c>
       <c r="I38">
         <f t="shared" si="3"/>
-        <v>849</v>
+        <v>277</v>
       </c>
       <c r="J38">
         <f t="shared" si="4"/>
-        <v>1268</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
@@ -1652,24 +1666,24 @@
       <c r="D39">
         <v>1497</v>
       </c>
-      <c r="F39">
-        <v>0</v>
+      <c r="F39" s="4">
+        <v>119</v>
       </c>
       <c r="G39">
         <f t="shared" si="1"/>
-        <v>1355</v>
+        <v>3587</v>
       </c>
       <c r="H39">
         <f t="shared" si="2"/>
-        <v>1796</v>
+        <v>1123</v>
       </c>
       <c r="I39">
         <f t="shared" si="3"/>
-        <v>496</v>
+        <v>1064</v>
       </c>
       <c r="J39">
         <f t="shared" si="4"/>
-        <v>1574</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
@@ -1685,24 +1699,24 @@
       <c r="D40">
         <v>1269</v>
       </c>
-      <c r="F40">
-        <v>19</v>
+      <c r="F40" s="4">
+        <v>185</v>
       </c>
       <c r="G40">
         <f t="shared" si="1"/>
-        <v>2346</v>
+        <v>3469</v>
       </c>
       <c r="H40">
         <f t="shared" si="2"/>
-        <v>573</v>
+        <v>1080</v>
       </c>
       <c r="I40">
         <f t="shared" si="3"/>
-        <v>1500</v>
+        <v>64</v>
       </c>
       <c r="J40">
         <f t="shared" si="4"/>
-        <v>988</v>
+        <v>321</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
@@ -1718,24 +1732,24 @@
       <c r="D41">
         <v>1599</v>
       </c>
-      <c r="F41">
-        <v>178</v>
+      <c r="F41" s="4">
+        <v>52</v>
       </c>
       <c r="G41">
         <f t="shared" si="1"/>
-        <v>3134</v>
+        <v>3166</v>
       </c>
       <c r="H41">
         <f t="shared" si="2"/>
-        <v>1169</v>
+        <v>973</v>
       </c>
       <c r="I41">
         <f t="shared" si="3"/>
-        <v>420</v>
+        <v>557</v>
       </c>
       <c r="J41">
         <f t="shared" si="4"/>
-        <v>1012</v>
+        <v>229</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
@@ -1751,24 +1765,24 @@
       <c r="D42">
         <v>1066</v>
       </c>
-      <c r="F42">
-        <v>164</v>
+      <c r="F42" s="4">
+        <v>57</v>
       </c>
       <c r="G42">
         <f t="shared" si="1"/>
-        <v>3842</v>
+        <v>3134</v>
       </c>
       <c r="H42">
         <f t="shared" si="2"/>
-        <v>1892</v>
+        <v>746</v>
       </c>
       <c r="I42">
         <f t="shared" si="3"/>
-        <v>597</v>
+        <v>555</v>
       </c>
       <c r="J42">
         <f t="shared" si="4"/>
-        <v>3557</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
@@ -1784,24 +1798,24 @@
       <c r="D43">
         <v>277</v>
       </c>
-      <c r="F43">
-        <v>159</v>
+      <c r="F43" s="4">
+        <v>92</v>
       </c>
       <c r="G43">
         <f t="shared" si="1"/>
-        <v>331</v>
+        <v>3174</v>
       </c>
       <c r="H43">
         <f t="shared" si="2"/>
-        <v>1322</v>
+        <v>606</v>
       </c>
       <c r="I43">
         <f t="shared" si="3"/>
-        <v>704</v>
+        <v>390</v>
       </c>
       <c r="J43">
         <f t="shared" si="4"/>
-        <v>1260</v>
+        <v>215</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
@@ -1817,24 +1831,24 @@
       <c r="D44">
         <v>379</v>
       </c>
-      <c r="F44">
-        <v>143</v>
+      <c r="F44" s="4">
+        <v>179</v>
       </c>
       <c r="G44">
         <f t="shared" si="1"/>
-        <v>1417</v>
+        <v>3369</v>
       </c>
       <c r="H44">
         <f t="shared" si="2"/>
-        <v>1961</v>
+        <v>697</v>
       </c>
       <c r="I44">
         <f t="shared" si="3"/>
-        <v>424</v>
+        <v>889</v>
       </c>
       <c r="J44">
         <f t="shared" si="4"/>
-        <v>1057</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
@@ -1850,24 +1864,24 @@
       <c r="D45">
         <v>158</v>
       </c>
-      <c r="F45">
-        <v>59</v>
+      <c r="F45" s="4">
+        <v>145</v>
       </c>
       <c r="G45">
         <f t="shared" si="1"/>
-        <v>1172</v>
+        <v>3400</v>
       </c>
       <c r="H45">
         <f t="shared" si="2"/>
-        <v>933</v>
+        <v>530</v>
       </c>
       <c r="I45">
         <f t="shared" si="3"/>
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="J45">
         <f t="shared" si="4"/>
-        <v>1074</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
@@ -1883,24 +1897,24 @@
       <c r="D46">
         <v>581</v>
       </c>
-      <c r="F46">
-        <v>147</v>
+      <c r="F46" s="4">
+        <v>78</v>
       </c>
       <c r="G46">
         <f t="shared" si="1"/>
-        <v>262</v>
+        <v>3399</v>
       </c>
       <c r="H46">
         <f t="shared" si="2"/>
-        <v>362</v>
+        <v>405</v>
       </c>
       <c r="I46">
         <f t="shared" si="3"/>
-        <v>1931</v>
+        <v>20</v>
       </c>
       <c r="J46">
         <f t="shared" si="4"/>
-        <v>775</v>
+        <v>309</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
@@ -1916,24 +1930,24 @@
       <c r="D47">
         <v>311</v>
       </c>
-      <c r="F47">
-        <v>116</v>
+      <c r="F47" s="4">
+        <v>31</v>
       </c>
       <c r="G47">
         <f t="shared" si="1"/>
-        <v>883</v>
+        <v>3697</v>
       </c>
       <c r="H47">
         <f t="shared" si="2"/>
-        <v>826</v>
+        <v>324</v>
       </c>
       <c r="I47">
         <f t="shared" si="3"/>
-        <v>345</v>
+        <v>394</v>
       </c>
       <c r="J47">
         <f t="shared" si="4"/>
-        <v>3169</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
@@ -1949,24 +1963,24 @@
       <c r="D48">
         <v>1867</v>
       </c>
-      <c r="F48">
-        <v>27</v>
+      <c r="F48" s="4">
+        <v>56</v>
       </c>
       <c r="G48">
         <f t="shared" si="1"/>
-        <v>3990</v>
+        <v>3796</v>
       </c>
       <c r="H48">
         <f t="shared" si="2"/>
-        <v>1450</v>
+        <v>244</v>
       </c>
       <c r="I48">
         <f t="shared" si="3"/>
-        <v>974</v>
+        <v>1046</v>
       </c>
       <c r="J48">
         <f t="shared" si="4"/>
-        <v>3349</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
@@ -1982,24 +1996,24 @@
       <c r="D49">
         <v>526</v>
       </c>
-      <c r="F49">
-        <v>96</v>
+      <c r="F49" s="4">
+        <v>113</v>
       </c>
       <c r="G49">
         <f t="shared" si="1"/>
-        <v>664</v>
+        <v>3819</v>
       </c>
       <c r="H49">
         <f t="shared" si="2"/>
-        <v>1058</v>
+        <v>191</v>
       </c>
       <c r="I49">
         <f t="shared" si="3"/>
-        <v>1278</v>
+        <v>283</v>
       </c>
       <c r="J49">
         <f t="shared" si="4"/>
-        <v>2805</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
@@ -2015,24 +2029,24 @@
       <c r="D50">
         <v>1188</v>
       </c>
-      <c r="F50">
-        <v>185</v>
+      <c r="F50" s="4">
+        <v>175</v>
       </c>
       <c r="G50">
         <f t="shared" si="1"/>
-        <v>3469</v>
+        <v>3828</v>
       </c>
       <c r="H50">
         <f t="shared" si="2"/>
-        <v>1080</v>
+        <v>57</v>
       </c>
       <c r="I50">
         <f t="shared" si="3"/>
-        <v>64</v>
+        <v>178</v>
       </c>
       <c r="J50">
         <f t="shared" si="4"/>
-        <v>1276</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
@@ -2048,24 +2062,24 @@
       <c r="D51">
         <v>986</v>
       </c>
-      <c r="F51">
-        <v>64</v>
+      <c r="F51" s="4">
+        <v>171</v>
       </c>
       <c r="G51">
         <f t="shared" si="1"/>
-        <v>2401</v>
+        <v>3726</v>
       </c>
       <c r="H51">
         <f t="shared" si="2"/>
-        <v>1778</v>
+        <v>56</v>
       </c>
       <c r="I51">
         <f t="shared" si="3"/>
-        <v>1685</v>
+        <v>237</v>
       </c>
       <c r="J51">
         <f t="shared" si="4"/>
-        <v>2368</v>
+        <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
@@ -2081,24 +2095,24 @@
       <c r="D52">
         <v>104</v>
       </c>
-      <c r="F52">
-        <v>20</v>
+      <c r="F52" s="4">
+        <v>16</v>
       </c>
       <c r="G52">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>3562</v>
       </c>
       <c r="H52">
         <f t="shared" si="2"/>
-        <v>1705</v>
+        <v>3</v>
       </c>
       <c r="I52">
         <f t="shared" si="3"/>
-        <v>1371</v>
+        <v>82</v>
       </c>
       <c r="J52">
         <f t="shared" si="4"/>
-        <v>3930</v>
+        <v>416</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
@@ -2114,24 +2128,24 @@
       <c r="D53">
         <v>1947</v>
       </c>
-      <c r="F53">
-        <v>71</v>
+      <c r="F53" s="4">
+        <v>25</v>
       </c>
       <c r="G53">
         <f t="shared" si="1"/>
-        <v>3964</v>
+        <v>3209</v>
       </c>
       <c r="H53">
         <f t="shared" si="2"/>
-        <v>1678</v>
+        <v>224</v>
       </c>
       <c r="I53">
         <f t="shared" si="3"/>
-        <v>1284</v>
+        <v>756</v>
       </c>
       <c r="J53">
         <f t="shared" si="4"/>
-        <v>1309</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
@@ -2147,24 +2161,24 @@
       <c r="D54">
         <v>617</v>
       </c>
-      <c r="F54">
-        <v>61</v>
+      <c r="F54" s="4">
+        <v>44</v>
       </c>
       <c r="G54">
         <f t="shared" si="1"/>
-        <v>2667</v>
+        <v>3134</v>
       </c>
       <c r="H54">
         <f t="shared" si="2"/>
-        <v>1503</v>
+        <v>177</v>
       </c>
       <c r="I54">
         <f t="shared" si="3"/>
-        <v>1995</v>
+        <v>311</v>
       </c>
       <c r="J54">
         <f t="shared" si="4"/>
-        <v>2151</v>
+        <v>522</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
@@ -2180,24 +2194,24 @@
       <c r="D55">
         <v>557</v>
       </c>
-      <c r="F55">
-        <v>163</v>
+      <c r="F55" s="4">
+        <v>75</v>
       </c>
       <c r="G55">
         <f t="shared" si="1"/>
-        <v>535</v>
+        <v>2614</v>
       </c>
       <c r="H55">
         <f t="shared" si="2"/>
-        <v>1791</v>
+        <v>132</v>
       </c>
       <c r="I55">
         <f t="shared" si="3"/>
-        <v>1423</v>
+        <v>360</v>
       </c>
       <c r="J55">
         <f t="shared" si="4"/>
-        <v>2379</v>
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
@@ -2213,24 +2227,24 @@
       <c r="D56">
         <v>81</v>
       </c>
-      <c r="F56">
-        <v>74</v>
+      <c r="F56" s="4">
+        <v>86</v>
       </c>
       <c r="G56">
         <f t="shared" si="1"/>
-        <v>2571</v>
+        <v>2398</v>
       </c>
       <c r="H56">
         <f t="shared" si="2"/>
-        <v>560</v>
+        <v>214</v>
       </c>
       <c r="I56">
         <f t="shared" si="3"/>
-        <v>1669</v>
+        <v>497</v>
       </c>
       <c r="J56">
         <f t="shared" si="4"/>
-        <v>1301</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
@@ -2246,24 +2260,24 @@
       <c r="D57">
         <v>557</v>
       </c>
-      <c r="F57">
-        <v>113</v>
+      <c r="F57" s="4">
+        <v>26</v>
       </c>
       <c r="G57">
         <f t="shared" si="1"/>
-        <v>3819</v>
+        <v>2371</v>
       </c>
       <c r="H57">
         <f t="shared" si="2"/>
-        <v>191</v>
+        <v>371</v>
       </c>
       <c r="I57">
         <f t="shared" si="3"/>
-        <v>283</v>
+        <v>834</v>
       </c>
       <c r="J57">
         <f t="shared" si="4"/>
-        <v>3755</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
@@ -2279,24 +2293,24 @@
       <c r="D58">
         <v>585</v>
       </c>
-      <c r="F58">
-        <v>195</v>
+      <c r="F58" s="4">
+        <v>100</v>
       </c>
       <c r="G58">
         <f t="shared" si="1"/>
-        <v>189</v>
+        <v>2343</v>
       </c>
       <c r="H58">
         <f t="shared" si="2"/>
-        <v>1151</v>
+        <v>360</v>
       </c>
       <c r="I58">
         <f t="shared" si="3"/>
-        <v>1145</v>
+        <v>965</v>
       </c>
       <c r="J58">
         <f t="shared" si="4"/>
-        <v>2090</v>
+        <v>253</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
@@ -2312,7 +2326,7 @@
       <c r="D59">
         <v>1046</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="4">
         <v>53</v>
       </c>
       <c r="G59">
@@ -2329,7 +2343,7 @@
       </c>
       <c r="J59">
         <f t="shared" si="4"/>
-        <v>1260</v>
+        <v>228</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
@@ -2345,24 +2359,24 @@
       <c r="D60">
         <v>555</v>
       </c>
-      <c r="F60">
-        <v>62</v>
+      <c r="F60" s="4">
+        <v>154</v>
       </c>
       <c r="G60">
         <f t="shared" si="1"/>
-        <v>2678</v>
+        <v>1878</v>
       </c>
       <c r="H60">
         <f t="shared" si="2"/>
-        <v>1417</v>
+        <v>234</v>
       </c>
       <c r="I60">
         <f t="shared" si="3"/>
-        <v>182</v>
+        <v>262</v>
       </c>
       <c r="J60">
         <f t="shared" si="4"/>
-        <v>459</v>
+        <v>87</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
@@ -2378,24 +2392,24 @@
       <c r="D61">
         <v>1284</v>
       </c>
-      <c r="F61">
-        <v>32</v>
+      <c r="F61" s="4">
+        <v>180</v>
       </c>
       <c r="G61">
         <f t="shared" si="1"/>
-        <v>3125</v>
+        <v>1913</v>
       </c>
       <c r="H61">
         <f t="shared" si="2"/>
-        <v>1312</v>
+        <v>314</v>
       </c>
       <c r="I61">
         <f t="shared" si="3"/>
-        <v>1585</v>
+        <v>175</v>
       </c>
       <c r="J61">
         <f t="shared" si="4"/>
-        <v>1570</v>
+        <v>302</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
@@ -2411,24 +2425,24 @@
       <c r="D62">
         <v>125</v>
       </c>
-      <c r="F62">
-        <v>180</v>
+      <c r="F62" s="4">
+        <v>135</v>
       </c>
       <c r="G62">
         <f t="shared" si="1"/>
-        <v>1913</v>
+        <v>1651</v>
       </c>
       <c r="H62">
         <f t="shared" si="2"/>
-        <v>314</v>
+        <v>164</v>
       </c>
       <c r="I62">
         <f t="shared" si="3"/>
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="J62">
         <f t="shared" si="4"/>
-        <v>2059</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.35">
@@ -2444,24 +2458,24 @@
       <c r="D63">
         <v>1686</v>
       </c>
-      <c r="F63">
-        <v>81</v>
+      <c r="F63" s="4">
+        <v>70</v>
       </c>
       <c r="G63">
         <f t="shared" si="1"/>
-        <v>3901</v>
+        <v>1639</v>
       </c>
       <c r="H63">
         <f t="shared" si="2"/>
-        <v>849</v>
+        <v>4</v>
       </c>
       <c r="I63">
         <f t="shared" si="3"/>
-        <v>606</v>
+        <v>622</v>
       </c>
       <c r="J63">
         <f t="shared" si="4"/>
-        <v>2114</v>
+        <v>346</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
@@ -2477,24 +2491,24 @@
       <c r="D64">
         <v>1995</v>
       </c>
-      <c r="F64">
-        <v>154</v>
+      <c r="F64" s="4">
+        <v>127</v>
       </c>
       <c r="G64">
         <f t="shared" si="1"/>
-        <v>1878</v>
+        <v>1311</v>
       </c>
       <c r="H64">
         <f t="shared" si="2"/>
-        <v>234</v>
+        <v>113</v>
       </c>
       <c r="I64">
         <f t="shared" si="3"/>
-        <v>262</v>
+        <v>736</v>
       </c>
       <c r="J64">
         <f t="shared" si="4"/>
-        <v>1535</v>
+        <v>237</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
@@ -2510,24 +2524,24 @@
       <c r="D65">
         <v>182</v>
       </c>
-      <c r="F65">
-        <v>102</v>
+      <c r="F65" s="4">
+        <v>123</v>
       </c>
       <c r="G65">
         <f t="shared" si="1"/>
-        <v>2866</v>
+        <v>1199</v>
       </c>
       <c r="H65">
         <f t="shared" si="2"/>
-        <v>1409</v>
+        <v>322</v>
       </c>
       <c r="I65">
         <f t="shared" si="3"/>
-        <v>939</v>
+        <v>119</v>
       </c>
       <c r="J65">
         <f t="shared" si="4"/>
-        <v>203</v>
+        <v>317</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
@@ -2543,24 +2557,24 @@
       <c r="D66">
         <v>129</v>
       </c>
-      <c r="F66">
-        <v>144</v>
+      <c r="F66" s="4">
+        <v>162</v>
       </c>
       <c r="G66">
         <f t="shared" si="1"/>
-        <v>2898</v>
+        <v>1416</v>
       </c>
       <c r="H66">
         <f t="shared" si="2"/>
-        <v>1609</v>
+        <v>553</v>
       </c>
       <c r="I66">
         <f t="shared" si="3"/>
-        <v>168</v>
+        <v>555</v>
       </c>
       <c r="J66">
         <f t="shared" si="4"/>
-        <v>1430</v>
+        <v>267</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
@@ -2576,24 +2590,24 @@
       <c r="D67">
         <v>1685</v>
       </c>
-      <c r="F67">
-        <v>141</v>
+      <c r="F67" s="4">
+        <v>133</v>
       </c>
       <c r="G67">
         <f t="shared" si="1"/>
-        <v>1521</v>
+        <v>1675</v>
       </c>
       <c r="H67">
         <f t="shared" si="2"/>
-        <v>1224</v>
+        <v>616</v>
       </c>
       <c r="I67">
         <f t="shared" si="3"/>
-        <v>1845</v>
+        <v>491</v>
       </c>
       <c r="J67">
         <f t="shared" si="4"/>
-        <v>1360</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
@@ -2609,24 +2623,24 @@
       <c r="D68">
         <v>163</v>
       </c>
-      <c r="F68">
-        <v>87</v>
+      <c r="F68" s="4">
+        <v>151</v>
       </c>
       <c r="G68">
         <f t="shared" ref="G68:G103" si="5">LOOKUP($F68,$A$3:$A$202,B$3:B$202)</f>
-        <v>2685</v>
+        <v>1525</v>
       </c>
       <c r="H68">
         <f t="shared" ref="H68:H103" si="6">LOOKUP($F68,$A$3:$A$202,C$3:C$202)</f>
-        <v>520</v>
+        <v>726</v>
       </c>
       <c r="I68">
         <f t="shared" ref="I68:I103" si="7">LOOKUP($F68,$A$3:$A$202,D$3:D$202)</f>
-        <v>1842</v>
+        <v>291</v>
       </c>
       <c r="J68">
         <f t="shared" ref="J68:J102" si="8">INT(SQRT((G68-G69)*(G68-G69)+(H68-H69)*(H68-H69)) +0.5)</f>
-        <v>849</v>
+        <v>304</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
@@ -2642,24 +2656,24 @@
       <c r="D69">
         <v>1604</v>
       </c>
-      <c r="F69">
-        <v>79</v>
+      <c r="F69" s="4">
+        <v>51</v>
       </c>
       <c r="G69">
         <f t="shared" si="5"/>
-        <v>1852</v>
+        <v>1479</v>
       </c>
       <c r="H69">
         <f t="shared" si="6"/>
-        <v>682</v>
+        <v>1027</v>
       </c>
       <c r="I69">
         <f t="shared" si="7"/>
-        <v>561</v>
+        <v>617</v>
       </c>
       <c r="J69">
         <f t="shared" si="8"/>
-        <v>528</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
@@ -2675,24 +2689,24 @@
       <c r="D70">
         <v>1688</v>
       </c>
-      <c r="F70">
-        <v>194</v>
+      <c r="F70" s="4">
+        <v>118</v>
       </c>
       <c r="G70">
         <f t="shared" si="5"/>
-        <v>1514</v>
+        <v>1229</v>
       </c>
       <c r="H70">
         <f t="shared" si="6"/>
-        <v>277</v>
+        <v>1036</v>
       </c>
       <c r="I70">
         <f t="shared" si="7"/>
-        <v>1340</v>
+        <v>824</v>
       </c>
       <c r="J70">
         <f t="shared" si="8"/>
-        <v>2454</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
@@ -2708,24 +2722,24 @@
       <c r="D71">
         <v>785</v>
       </c>
-      <c r="F71">
-        <v>21</v>
+      <c r="F71" s="4">
+        <v>59</v>
       </c>
       <c r="G71">
         <f t="shared" si="5"/>
-        <v>3365</v>
+        <v>1172</v>
       </c>
       <c r="H71">
         <f t="shared" si="6"/>
-        <v>1888</v>
+        <v>933</v>
       </c>
       <c r="I71">
         <f t="shared" si="7"/>
-        <v>774</v>
+        <v>125</v>
       </c>
       <c r="J71">
         <f t="shared" si="8"/>
-        <v>1867</v>
+        <v>287</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.35">
@@ -2741,24 +2755,24 @@
       <c r="D72">
         <v>1033</v>
       </c>
-      <c r="F72">
-        <v>171</v>
+      <c r="F72" s="4">
+        <v>65</v>
       </c>
       <c r="G72">
         <f t="shared" si="5"/>
-        <v>3726</v>
+        <v>928</v>
       </c>
       <c r="H72">
         <f t="shared" si="6"/>
-        <v>56</v>
+        <v>782</v>
       </c>
       <c r="I72">
         <f t="shared" si="7"/>
-        <v>237</v>
+        <v>163</v>
       </c>
       <c r="J72">
         <f t="shared" si="8"/>
-        <v>3851</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
@@ -2774,24 +2788,24 @@
       <c r="D73">
         <v>622</v>
       </c>
-      <c r="F73">
-        <v>108</v>
+      <c r="F73" s="4">
+        <v>116</v>
       </c>
       <c r="G73">
         <f t="shared" si="5"/>
-        <v>389</v>
+        <v>883</v>
       </c>
       <c r="H73">
         <f t="shared" si="6"/>
-        <v>1979</v>
+        <v>826</v>
       </c>
       <c r="I73">
         <f t="shared" si="7"/>
-        <v>686</v>
+        <v>345</v>
       </c>
       <c r="J73">
         <f t="shared" si="8"/>
-        <v>2083</v>
+        <v>170</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.35">
@@ -2807,24 +2821,24 @@
       <c r="D74">
         <v>1284</v>
       </c>
-      <c r="F74">
-        <v>15</v>
+      <c r="F74" s="4">
+        <v>43</v>
       </c>
       <c r="G74">
         <f t="shared" si="5"/>
-        <v>2428</v>
+        <v>724</v>
       </c>
       <c r="H74">
         <f t="shared" si="6"/>
-        <v>1551</v>
+        <v>765</v>
       </c>
       <c r="I74">
         <f t="shared" si="7"/>
-        <v>891</v>
+        <v>581</v>
       </c>
       <c r="J74">
         <f t="shared" si="8"/>
-        <v>1292</v>
+        <v>375</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
@@ -2840,24 +2854,24 @@
       <c r="D75">
         <v>1284</v>
       </c>
-      <c r="F75">
-        <v>117</v>
+      <c r="F75" s="4">
+        <v>184</v>
       </c>
       <c r="G75">
         <f t="shared" si="5"/>
-        <v>1199</v>
+        <v>518</v>
       </c>
       <c r="H75">
         <f t="shared" si="6"/>
-        <v>1948</v>
+        <v>452</v>
       </c>
       <c r="I75">
         <f t="shared" si="7"/>
-        <v>611</v>
+        <v>296</v>
       </c>
       <c r="J75">
         <f t="shared" si="8"/>
-        <v>1303</v>
+        <v>232</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
@@ -2873,24 +2887,24 @@
       <c r="D76">
         <v>1390</v>
       </c>
-      <c r="F76">
-        <v>22</v>
+      <c r="F76" s="4">
+        <v>35</v>
       </c>
       <c r="G76">
         <f t="shared" si="5"/>
-        <v>47</v>
+        <v>729</v>
       </c>
       <c r="H76">
         <f t="shared" si="6"/>
-        <v>1340</v>
+        <v>356</v>
       </c>
       <c r="I76">
         <f t="shared" si="7"/>
-        <v>88</v>
+        <v>976</v>
       </c>
       <c r="J76">
         <f t="shared" si="8"/>
-        <v>3125</v>
+        <v>149</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
@@ -2906,24 +2920,24 @@
       <c r="D77">
         <v>1669</v>
       </c>
-      <c r="F77">
-        <v>55</v>
+      <c r="F77" s="4">
+        <v>84</v>
       </c>
       <c r="G77">
         <f t="shared" si="5"/>
-        <v>3144</v>
+        <v>656</v>
       </c>
       <c r="H77">
         <f t="shared" si="6"/>
-        <v>924</v>
+        <v>226</v>
       </c>
       <c r="I77">
         <f t="shared" si="7"/>
-        <v>585</v>
+        <v>931</v>
       </c>
       <c r="J77">
         <f t="shared" si="8"/>
-        <v>2567</v>
+        <v>215</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
@@ -2939,24 +2953,24 @@
       <c r="D78">
         <v>360</v>
       </c>
-      <c r="F78">
-        <v>36</v>
+      <c r="F78" s="4">
+        <v>112</v>
       </c>
       <c r="G78">
         <f t="shared" si="5"/>
-        <v>771</v>
+        <v>816</v>
       </c>
       <c r="H78">
         <f t="shared" si="6"/>
-        <v>1904</v>
+        <v>83</v>
       </c>
       <c r="I78">
         <f t="shared" si="7"/>
-        <v>1497</v>
+        <v>607</v>
       </c>
       <c r="J78">
         <f t="shared" si="8"/>
-        <v>2189</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.35">
@@ -2972,24 +2986,24 @@
       <c r="D79">
         <v>1888</v>
       </c>
-      <c r="F79">
-        <v>132</v>
+      <c r="F79" s="4">
+        <v>4</v>
       </c>
       <c r="G79">
         <f t="shared" si="5"/>
-        <v>2959</v>
+        <v>661</v>
       </c>
       <c r="H79">
         <f t="shared" si="6"/>
-        <v>1856</v>
+        <v>87</v>
       </c>
       <c r="I79">
         <f t="shared" si="7"/>
-        <v>1792</v>
+        <v>903</v>
       </c>
       <c r="J79">
         <f t="shared" si="8"/>
-        <v>814</v>
+        <v>288</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
@@ -3005,24 +3019,24 @@
       <c r="D80">
         <v>1351</v>
       </c>
-      <c r="F80">
-        <v>128</v>
+      <c r="F80" s="4">
+        <v>190</v>
       </c>
       <c r="G80">
         <f t="shared" si="5"/>
-        <v>2759</v>
+        <v>373</v>
       </c>
       <c r="H80">
         <f t="shared" si="6"/>
-        <v>1067</v>
+        <v>80</v>
       </c>
       <c r="I80">
         <f t="shared" si="7"/>
-        <v>1588</v>
+        <v>931</v>
       </c>
       <c r="J80">
         <f t="shared" si="8"/>
-        <v>1119</v>
+        <v>128</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
@@ -3038,24 +3052,24 @@
       <c r="D81">
         <v>20</v>
       </c>
-      <c r="F81">
-        <v>76</v>
+      <c r="F81" s="4">
+        <v>10</v>
       </c>
       <c r="G81">
         <f t="shared" si="5"/>
-        <v>1842</v>
+        <v>249</v>
       </c>
       <c r="H81">
         <f t="shared" si="6"/>
-        <v>1709</v>
+        <v>47</v>
       </c>
       <c r="I81">
         <f t="shared" si="7"/>
-        <v>1888</v>
+        <v>774</v>
       </c>
       <c r="J81">
         <f t="shared" si="8"/>
-        <v>1309</v>
+        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
@@ -3071,24 +3085,24 @@
       <c r="D82">
         <v>561</v>
       </c>
-      <c r="F82">
-        <v>161</v>
+      <c r="F82" s="4">
+        <v>177</v>
       </c>
       <c r="G82">
         <f t="shared" si="5"/>
-        <v>1414</v>
+        <v>263</v>
       </c>
       <c r="H82">
         <f t="shared" si="6"/>
-        <v>472</v>
+        <v>208</v>
       </c>
       <c r="I82">
         <f t="shared" si="7"/>
-        <v>1719</v>
+        <v>527</v>
       </c>
       <c r="J82">
         <f t="shared" si="8"/>
-        <v>1349</v>
+        <v>261</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
@@ -3104,24 +3118,24 @@
       <c r="D83">
         <v>445</v>
       </c>
-      <c r="F83">
-        <v>153</v>
+      <c r="F83" s="4">
+        <v>30</v>
       </c>
       <c r="G83">
         <f t="shared" si="5"/>
-        <v>1508</v>
+        <v>97</v>
       </c>
       <c r="H83">
         <f t="shared" si="6"/>
-        <v>1818</v>
+        <v>409</v>
       </c>
       <c r="I83">
         <f t="shared" si="7"/>
-        <v>1287</v>
+        <v>1025</v>
       </c>
       <c r="J83">
         <f t="shared" si="8"/>
-        <v>2789</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
@@ -3137,24 +3151,24 @@
       <c r="D84">
         <v>606</v>
       </c>
-      <c r="F84">
-        <v>88</v>
+      <c r="F84" s="4">
+        <v>54</v>
       </c>
       <c r="G84">
         <f t="shared" si="5"/>
-        <v>3626</v>
+        <v>165</v>
       </c>
       <c r="H84">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>413</v>
       </c>
       <c r="I84">
         <f t="shared" si="7"/>
-        <v>1866</v>
+        <v>557</v>
       </c>
       <c r="J84">
         <f t="shared" si="8"/>
-        <v>2318</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
@@ -3170,24 +3184,24 @@
       <c r="D85">
         <v>1133</v>
       </c>
-      <c r="F85">
-        <v>127</v>
+      <c r="F85" s="4">
+        <v>48</v>
       </c>
       <c r="G85">
         <f t="shared" si="5"/>
-        <v>1311</v>
+        <v>227</v>
       </c>
       <c r="H85">
         <f t="shared" si="6"/>
-        <v>113</v>
+        <v>534</v>
       </c>
       <c r="I85">
         <f t="shared" si="7"/>
-        <v>736</v>
+        <v>986</v>
       </c>
       <c r="J85">
         <f t="shared" si="8"/>
-        <v>1729</v>
+        <v>159</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
@@ -3203,24 +3217,24 @@
       <c r="D86">
         <v>1899</v>
       </c>
-      <c r="F86">
-        <v>186</v>
+      <c r="F86" s="4">
+        <v>160</v>
       </c>
       <c r="G86">
         <f t="shared" si="5"/>
-        <v>2121</v>
+        <v>307</v>
       </c>
       <c r="H86">
         <f t="shared" si="6"/>
-        <v>1641</v>
+        <v>671</v>
       </c>
       <c r="I86">
         <f t="shared" si="7"/>
-        <v>859</v>
+        <v>228</v>
       </c>
       <c r="J86">
         <f t="shared" si="8"/>
-        <v>1237</v>
+        <v>282</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
@@ -3236,24 +3250,24 @@
       <c r="D87">
         <v>931</v>
       </c>
-      <c r="F87">
-        <v>45</v>
+      <c r="F87" s="4">
+        <v>34</v>
       </c>
       <c r="G87">
         <f t="shared" si="5"/>
-        <v>1450</v>
+        <v>43</v>
       </c>
       <c r="H87">
         <f t="shared" si="6"/>
-        <v>602</v>
+        <v>770</v>
       </c>
       <c r="I87">
         <f t="shared" si="7"/>
-        <v>1867</v>
+        <v>191</v>
       </c>
       <c r="J87">
         <f t="shared" si="8"/>
-        <v>1290</v>
+        <v>378</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
@@ -3269,24 +3283,24 @@
       <c r="D88">
         <v>1618</v>
       </c>
-      <c r="F88">
-        <v>167</v>
+      <c r="F88" s="4">
+        <v>146</v>
       </c>
       <c r="G88">
         <f t="shared" si="5"/>
-        <v>2682</v>
+        <v>60</v>
       </c>
       <c r="H88">
         <f t="shared" si="6"/>
-        <v>984</v>
+        <v>1148</v>
       </c>
       <c r="I88">
         <f t="shared" si="7"/>
-        <v>960</v>
+        <v>839</v>
       </c>
       <c r="J88">
         <f t="shared" si="8"/>
-        <v>705</v>
+        <v>192</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
@@ -3302,24 +3316,24 @@
       <c r="D89">
         <v>497</v>
       </c>
-      <c r="F89">
-        <v>101</v>
+      <c r="F89" s="4">
+        <v>22</v>
       </c>
       <c r="G89">
         <f t="shared" si="5"/>
-        <v>2504</v>
+        <v>47</v>
       </c>
       <c r="H89">
         <f t="shared" si="6"/>
-        <v>302</v>
+        <v>1340</v>
       </c>
       <c r="I89">
         <f t="shared" si="7"/>
-        <v>297</v>
+        <v>88</v>
       </c>
       <c r="J89">
         <f t="shared" si="8"/>
-        <v>319</v>
+        <v>539</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
@@ -3335,24 +3349,24 @@
       <c r="D90">
         <v>1842</v>
       </c>
-      <c r="F90">
-        <v>99</v>
+      <c r="F90" s="4">
+        <v>18</v>
       </c>
       <c r="G90">
         <f t="shared" si="5"/>
-        <v>2246</v>
+        <v>229</v>
       </c>
       <c r="H90">
         <f t="shared" si="6"/>
-        <v>490</v>
+        <v>1847</v>
       </c>
       <c r="I90">
         <f t="shared" si="7"/>
-        <v>1895</v>
+        <v>182</v>
       </c>
       <c r="J90">
         <f t="shared" si="8"/>
-        <v>678</v>
+        <v>207</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
@@ -3368,24 +3382,24 @@
       <c r="D91">
         <v>1866</v>
       </c>
-      <c r="F91">
-        <v>135</v>
+      <c r="F91" s="4">
+        <v>108</v>
       </c>
       <c r="G91">
         <f t="shared" si="5"/>
-        <v>1651</v>
+        <v>389</v>
       </c>
       <c r="H91">
         <f t="shared" si="6"/>
-        <v>164</v>
+        <v>1979</v>
       </c>
       <c r="I91">
         <f t="shared" si="7"/>
-        <v>197</v>
+        <v>686</v>
       </c>
       <c r="J91">
         <f t="shared" si="8"/>
-        <v>880</v>
+        <v>142</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.35">
@@ -3401,24 +3415,24 @@
       <c r="D92">
         <v>754</v>
       </c>
-      <c r="F92">
-        <v>51</v>
+      <c r="F92" s="4">
+        <v>69</v>
       </c>
       <c r="G92">
         <f t="shared" si="5"/>
-        <v>1479</v>
+        <v>359</v>
       </c>
       <c r="H92">
         <f t="shared" si="6"/>
-        <v>1027</v>
+        <v>1840</v>
       </c>
       <c r="I92">
         <f t="shared" si="7"/>
-        <v>617</v>
+        <v>1033</v>
       </c>
       <c r="J92">
         <f t="shared" si="8"/>
-        <v>1154</v>
+        <v>519</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.35">
@@ -3434,24 +3448,24 @@
       <c r="D93">
         <v>246</v>
       </c>
-      <c r="F93">
-        <v>112</v>
+      <c r="F93" s="4">
+        <v>159</v>
       </c>
       <c r="G93">
         <f t="shared" si="5"/>
-        <v>816</v>
+        <v>331</v>
       </c>
       <c r="H93">
         <f t="shared" si="6"/>
-        <v>83</v>
+        <v>1322</v>
       </c>
       <c r="I93">
         <f t="shared" si="7"/>
-        <v>607</v>
+        <v>704</v>
       </c>
       <c r="J93">
         <f t="shared" si="8"/>
-        <v>1330</v>
+        <v>368</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.35">
@@ -3467,24 +3481,24 @@
       <c r="D94">
         <v>1510</v>
       </c>
-      <c r="F94">
-        <v>66</v>
+      <c r="F94" s="4">
+        <v>181</v>
       </c>
       <c r="G94">
         <f t="shared" si="5"/>
-        <v>1642</v>
+        <v>314</v>
       </c>
       <c r="H94">
         <f t="shared" si="6"/>
-        <v>1125</v>
+        <v>954</v>
       </c>
       <c r="I94">
         <f t="shared" si="7"/>
-        <v>1604</v>
+        <v>736</v>
       </c>
       <c r="J94">
         <f t="shared" si="8"/>
-        <v>946</v>
+        <v>275</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.35">
@@ -3500,24 +3514,24 @@
       <c r="D95">
         <v>390</v>
       </c>
-      <c r="F95">
-        <v>6</v>
+      <c r="F95" s="4">
+        <v>42</v>
       </c>
       <c r="G95">
         <f t="shared" si="5"/>
-        <v>1748</v>
+        <v>583</v>
       </c>
       <c r="H95">
         <f t="shared" si="6"/>
-        <v>185</v>
+        <v>895</v>
       </c>
       <c r="I95">
         <f t="shared" si="7"/>
-        <v>1859</v>
+        <v>158</v>
       </c>
       <c r="J95">
         <f t="shared" si="8"/>
-        <v>830</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.35">
@@ -3533,24 +3547,24 @@
       <c r="D96">
         <v>860</v>
       </c>
-      <c r="F96">
-        <v>156</v>
+      <c r="F96" s="4">
+        <v>5</v>
       </c>
       <c r="G96">
         <f t="shared" si="5"/>
-        <v>932</v>
+        <v>628</v>
       </c>
       <c r="H96">
         <f t="shared" si="6"/>
-        <v>34</v>
+        <v>974</v>
       </c>
       <c r="I96">
         <f t="shared" si="7"/>
-        <v>1625</v>
+        <v>1081</v>
       </c>
       <c r="J96">
         <f t="shared" si="8"/>
-        <v>3090</v>
+        <v>347</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.35">
@@ -3566,24 +3580,24 @@
       <c r="D97">
         <v>323</v>
       </c>
-      <c r="F97">
-        <v>98</v>
+      <c r="F97" s="4">
+        <v>115</v>
       </c>
       <c r="G97">
         <f t="shared" si="5"/>
-        <v>3954</v>
+        <v>893</v>
       </c>
       <c r="H97">
         <f t="shared" si="6"/>
-        <v>681</v>
+        <v>1198</v>
       </c>
       <c r="I97">
         <f t="shared" si="7"/>
-        <v>1727</v>
+        <v>166</v>
       </c>
       <c r="J97">
         <f t="shared" si="8"/>
-        <v>3631</v>
+        <v>346</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.35">
@@ -3599,24 +3613,24 @@
       <c r="D98">
         <v>1075</v>
       </c>
-      <c r="F98">
-        <v>190</v>
+      <c r="F98" s="4">
+        <v>41</v>
       </c>
       <c r="G98">
         <f t="shared" si="5"/>
-        <v>373</v>
+        <v>550</v>
       </c>
       <c r="H98">
         <f t="shared" si="6"/>
-        <v>80</v>
+        <v>1241</v>
       </c>
       <c r="I98">
         <f t="shared" si="7"/>
-        <v>931</v>
+        <v>379</v>
       </c>
       <c r="J98">
         <f t="shared" si="8"/>
-        <v>1233</v>
+        <v>69</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.35">
@@ -3632,24 +3646,24 @@
       <c r="D99">
         <v>1278</v>
       </c>
-      <c r="F99">
-        <v>72</v>
+      <c r="F99" s="4">
+        <v>193</v>
       </c>
       <c r="G99">
         <f t="shared" si="5"/>
-        <v>1341</v>
+        <v>501</v>
       </c>
       <c r="H99">
         <f t="shared" si="6"/>
-        <v>844</v>
+        <v>1290</v>
       </c>
       <c r="I99">
         <f t="shared" si="7"/>
-        <v>1284</v>
+        <v>5</v>
       </c>
       <c r="J99">
         <f t="shared" si="8"/>
-        <v>900</v>
+        <v>301</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.35">
@@ -3665,24 +3679,24 @@
       <c r="D100">
         <v>310</v>
       </c>
-      <c r="F100">
-        <v>94</v>
+      <c r="F100" s="4">
+        <v>139</v>
       </c>
       <c r="G100">
         <f t="shared" si="5"/>
-        <v>2237</v>
+        <v>772</v>
       </c>
       <c r="H100">
         <f t="shared" si="6"/>
-        <v>764</v>
+        <v>1422</v>
       </c>
       <c r="I100">
         <f t="shared" si="7"/>
-        <v>323</v>
+        <v>150</v>
       </c>
       <c r="J100">
         <f t="shared" si="8"/>
-        <v>201</v>
+        <v>270</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">
@@ -3698,24 +3712,24 @@
       <c r="D101">
         <v>1727</v>
       </c>
-      <c r="F101">
-        <v>12</v>
+      <c r="F101" s="4">
+        <v>68</v>
       </c>
       <c r="G101">
         <f t="shared" si="5"/>
-        <v>2219</v>
+        <v>922</v>
       </c>
       <c r="H101">
         <f t="shared" si="6"/>
-        <v>964</v>
+        <v>1647</v>
       </c>
       <c r="I101">
         <f t="shared" si="7"/>
-        <v>1370</v>
+        <v>785</v>
       </c>
       <c r="J101">
         <f t="shared" si="8"/>
-        <v>1107</v>
+        <v>243</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.35">
@@ -3731,24 +3745,24 @@
       <c r="D102">
         <v>1895</v>
       </c>
-      <c r="F102">
-        <v>73</v>
+      <c r="F102" s="4">
+        <v>46</v>
       </c>
       <c r="G102">
         <f t="shared" si="5"/>
-        <v>2791</v>
+        <v>1065</v>
       </c>
       <c r="H102">
         <f t="shared" si="6"/>
-        <v>1912</v>
+        <v>1451</v>
       </c>
       <c r="I102">
         <f t="shared" si="7"/>
-        <v>1390</v>
+        <v>526</v>
       </c>
       <c r="J102">
         <f t="shared" si="8"/>
-        <v>1828</v>
+        <v>451</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.35">
@@ -3766,19 +3780,19 @@
       </c>
       <c r="F103">
         <f>F3</f>
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="G103">
         <f t="shared" si="5"/>
-        <v>3697</v>
+        <v>1355</v>
       </c>
       <c r="H103">
         <f t="shared" si="6"/>
-        <v>324</v>
+        <v>1796</v>
       </c>
       <c r="I103">
         <f t="shared" si="7"/>
-        <v>394</v>
+        <v>496</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.35">
@@ -5177,8 +5191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>